<commit_message>
eRST utils for GENTLE
</commit_message>
<xml_diff>
--- a/_build/utils/dm-dependencies/resources/non_dm_rules.xlsx
+++ b/_build/utils/dm-dependencies/resources/non_dm_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Corpora\GUM\GENTLE\repo\_build\utils\dm-dependencies\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDAEDFB-A943-4115-933F-064A16C4C123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA5E7FB-EAC6-473B-B4D4-80D6A72D127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BF4EFA19-1866-4339-A4F4-33A768915554}"/>
   </bookViews>
@@ -898,9 +898,6 @@
     <t>now</t>
   </si>
   <si>
-    <t>(love|hope|feel|look|seem|appreciate|regret|suck|sound|thank|support|surprise|resonate|mean|hate|like|sigh|agree|alarm|amaze|enjoy|frown|applaud|believe|welcome|honor|honour|matter|advise|laugh)</t>
-  </si>
-  <si>
     <t>(not|never)</t>
   </si>
   <si>
@@ -994,9 +991,6 @@
     <t>(aim|purpose|goal|achieve|prevent|stop|avoid|eliminate)</t>
   </si>
   <si>
-    <t>gram=(laid_-_back|self_-_loathing|within_our_reach|can_not_wait|mind_blowing|sore_spot|must_be|freak_out|no_choice)_</t>
-  </si>
-  <si>
     <t>Numerical=Yes</t>
   </si>
   <si>
@@ -1012,18 +1006,12 @@
     <t>(consider|P\.?S\.?|sincerely)</t>
   </si>
   <si>
-    <t>$attrib_verb = (accept|acknowledge|add|admit|afraid|agree|announce|argue|ask|assert|assess|assume|assure|aware|believe|bet|call|certain|chant|check|claim|comment|complain|concern|conclude|confirm|convince|cry|decide|declare|determine|disappoint|discover|discuss|doubt|dream|emphasize|ensure|establish|estimate|exclaim|expect|explain|express|feel|figure|find|forget|gather|glad|guess|happy|hear|hope|hypothesize|imagine|imply|indicate|inform|know|learn|lie|maintain|mean|mention|mindful|note|notice|observe|pant|perceive|point|posit|pray|predict|presume|promise|propose|proud|quote|re-iterate|read|realise|realize|reason|recall|recognize|recommend|reiterate|remember|remind|reply|report|resent|reveal|rule|say|scream|see|shout|show|shrug|sing|snap|start|state|suggest|summarize|suppose|sure|surprise|surprised|suspect|swear|tell|terrify|think|tweet|understand|vlog|whisper|wish|witness|wonder|worry|write|be%like|go%say|keep%mind|bear%mind|make%sure)</t>
-  </si>
-  <si>
     <t>gram=(result_from|owe_to|as_such|that_make|give_rise|lead_to)_</t>
   </si>
   <si>
     <t>gram=(in_response|lead_to)_</t>
   </si>
   <si>
-    <t>(accurate|amazing|attractive|awesome|awful|bad|beautiful|big|cathartic|cautionary|clear|complicated|considerable|cool|correct|crazy|critical|cute|dark|decent|different|difficult|dreadful|easy|efficient|enough|essential|excellent|excited|exciting|false|fantastic|fine|frightful|froughtful|fun|fundamental|funny|glad|goddamn|good|great|gross|happy|hard|heady|healthy|heartwarming|high|historic|honest|ideal|important|inaccurate|insane|interesting|large|legendary|likely|long|low|lucky|magnificent|militant|natural|necessary|needy|nice|normal|okay|peaceful|perfect|pleasant|possible|practical|pretty|proud|rare|real|realistic|reliable|remarkable|right|sad|safe|same|scared|scary|scenic|significant|small|smart|sorry|special|strange|strong|stupid|sure|surprising|sweet|tame|tired|toxic|trash|tremendous|true|unlikely|unpalatable|unprecedented|useful|valuable|versatile|warm|weird|wild|wild|wonderful|worth|wrong)</t>
-  </si>
-  <si>
     <t>(yes|no|yeah|right|yup|nope)</t>
   </si>
   <si>
@@ -1039,10 +1027,22 @@
     <t>(?i)(considering)</t>
   </si>
   <si>
-    <t>(importantly|shit|fun|loser|probably|strangely|oddly|fuck|hopefully|fortunately|unfortunately|fucking|proble-|problem|lol|oWo|:/|:\)|:\(|;\)|best|:-\)|:-\(|interestingly|striking|very|extremely|highly|exceptionally|extraordinarily|masterpiece|top|milestone|sadness|excitement|ew|yikes|yay|whoa|delight|hard|legend)</t>
-  </si>
-  <si>
     <t>First=EDU</t>
+  </si>
+  <si>
+    <t>gram=(can_not_wait|ca_n't_wait|commanding_lead|God_forbid|laid_-_back|mind_blowing|must_be|self_-_loathing|should_have|sore_spot|stacks_up|within_our_reach|freak_out|no_choice|no_joke)_</t>
+  </si>
+  <si>
+    <t>(advise|feel|love|hope|kid|look|seem|appreciate|regret|suck|sound|thank|support|surprise|resonate|mean|hate|like|sigh|agree|alarm|amaze|enjoy|frown|applaud|believe|welcome|honor|honour|matter|laugh|marvel)</t>
+  </si>
+  <si>
+    <t>(BS|doubtless|evil|fortunately|fuck|fucking|fun|hopefully|importantly|loser|oddly|probably|shit|strangely|top|justly|unfortunately|pissed|proble-|problem|lol|oWo|:/|:\)|:\(|;\)|best|:-\)|:-\(|interestingly|striking|very|extremely|highly|exceptionally|extraordinarily|masterpiece|top|milestone|sadness|excitement|ew|yikes|yay|whoa|delight|hard|legend|yes)</t>
+  </si>
+  <si>
+    <t>$attrib_verb = (accept|acknowledge|add|admit|afraid|agree|announce|argue|ask|assert|assess|assume|assure|aware|believe|bet|call|care|certain|chant|check|claim|comment|complain|concern|conclude|confirm|convince|cry|decide|declare|determine|disappoint|discover|discuss|doubt|dream|emphasize|ensure|establish|estimate|exclaim|expect|explain|express|feel|figure|find|forget|gather|glad|guarantee|guess|happy|hear|hold|hope|hypothesize|imagine|implore|imply|indicate|inform|know|learn|lie|maintain|mean|mention|mindful|mutter|note|notice|observe|pant|perceive|point|posit|pray|predict|presume|promise|propose|proud|quote|quoth|re-iterate|read|realise|realize|reason|recall|recognize|recommend|reiterate|remember|remind|repeat|reply|report|resent|reveal|rule|say|scream|see|shout|show|shriek|shrug|sing|snap|start|state|stunned|suggest|summarize|suppose|sure|surprise|surprised|suspect|swear|tell|terrify|think|trust|tweet|understand|vlog|whisper|wish|witness|wonder|worry|write|be%like|go%say|keep%mind|bear%mind|make%sure)</t>
+  </si>
+  <si>
+    <t>(accurate|aggressive|amaze|amazing|attractive|awesome|awful|bad|beautiful|big|cathartic|cautionary|clean|clear|complicated|considerable|cool|correct|crazy|critical|cute|dark|decent|different|difficult|dreadful|easy|efficient|enough|essential|excellent|excited|exciting|false|fantastic|fine|frightful|froughtful|frustrate|fun|fundamental|funny|glad|goddamn|good|great|gross|happy|hard|heady|healthy|heartwarming|high|historic|honest|ideal|important|inaccurate|incorrect|insane|interesting|large|legendary|likely|long|low|lucky|magnificent|militant|natural|necessary|needy|nice|normal|okay|peaceful|perfect|pleasant|possible|practical|pretty|proud|rare|real|realistic|reliable|remarkable|right|sad|safe|same|scared|scary|scenic|significant|simple|small|smart|solid|sorry|special|strange|strong|stun|stunned|stupid|sure|surpries|surprising|sweet|tame|tired|toxic|trash|tremendous|true|unbelievable|unlikely|unnatural|unpalatable|unprecedented|useful|valuable|versatile|violent|warm|weird|wild|wild|wonderful|worth|wrong)</t>
   </si>
 </sst>
 </file>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFA5BF6-386C-4E06-8AEF-60CB8C63BD33}">
   <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S114" sqref="S114"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -1659,13 +1659,13 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
         <v>314</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>315</v>
       </c>
       <c r="F8" t="s">
         <v>88</v>
@@ -1674,7 +1674,7 @@
         <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I8" t="s">
         <v>55</v>
@@ -1707,7 +1707,7 @@
         <v>12</v>
       </c>
       <c r="S8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -1916,7 +1916,7 @@
         <v>55</v>
       </c>
       <c r="J12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K12" t="s">
         <v>55</v>
@@ -1925,7 +1925,7 @@
         <v>55</v>
       </c>
       <c r="M12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N12" t="s">
         <v>55</v>
@@ -1960,7 +1960,7 @@
         <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F13" t="s">
         <v>55</v>
@@ -1975,7 +1975,7 @@
         <v>55</v>
       </c>
       <c r="J13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K13" t="s">
         <v>55</v>
@@ -1984,7 +1984,7 @@
         <v>55</v>
       </c>
       <c r="M13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N13" t="s">
         <v>55</v>
@@ -1996,13 +1996,13 @@
         <v>13</v>
       </c>
       <c r="Q13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R13" t="s">
         <v>12</v>
       </c>
       <c r="S13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2013,7 +2013,7 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="D14" t="s">
         <v>55</v>
@@ -2072,7 +2072,7 @@
         <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>290</v>
+        <v>335</v>
       </c>
       <c r="D15" t="s">
         <v>55</v>
@@ -2131,7 +2131,7 @@
         <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D16" t="s">
         <v>55</v>
@@ -2190,7 +2190,7 @@
         <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D17" t="s">
         <v>55</v>
@@ -2232,7 +2232,7 @@
         <v>38</v>
       </c>
       <c r="Q17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R17" t="s">
         <v>12</v>
@@ -2323,13 +2323,13 @@
         <v>55</v>
       </c>
       <c r="H19" t="s">
+        <v>317</v>
+      </c>
+      <c r="I19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" t="s">
         <v>318</v>
-      </c>
-      <c r="I19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" t="s">
-        <v>319</v>
       </c>
       <c r="K19" t="s">
         <v>55</v>
@@ -2506,10 +2506,10 @@
         <v>55</v>
       </c>
       <c r="J22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L22" t="s">
         <v>55</v>
@@ -2533,7 +2533,7 @@
         <v>12</v>
       </c>
       <c r="S22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
@@ -2541,7 +2541,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C23" t="s">
         <v>55</v>
@@ -2839,7 +2839,7 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D28" t="s">
         <v>55</v>
@@ -3037,7 +3037,7 @@
         <v>55</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K31" t="s">
         <v>55</v>
@@ -3311,7 +3311,7 @@
         <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D36" t="s">
         <v>55</v>
@@ -3547,7 +3547,7 @@
         <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D40" t="s">
         <v>55</v>
@@ -3595,7 +3595,7 @@
         <v>12</v>
       </c>
       <c r="S40" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
@@ -4255,7 +4255,7 @@
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D52" t="s">
         <v>55</v>
@@ -4323,7 +4323,7 @@
         <v>55</v>
       </c>
       <c r="F53" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G53" t="s">
         <v>55</v>
@@ -4362,7 +4362,7 @@
         <v>12</v>
       </c>
       <c r="S53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.35">
@@ -4807,7 +4807,7 @@
         <v>55</v>
       </c>
       <c r="J61" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="K61" t="s">
         <v>55</v>
@@ -5515,7 +5515,7 @@
         <v>55</v>
       </c>
       <c r="J73" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K73" t="s">
         <v>55</v>
@@ -6105,7 +6105,7 @@
         <v>55</v>
       </c>
       <c r="J83" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="K83" t="s">
         <v>55</v>
@@ -6497,7 +6497,7 @@
         <v>55</v>
       </c>
       <c r="C90" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D90" t="s">
         <v>55</v>
@@ -6556,7 +6556,7 @@
         <v>55</v>
       </c>
       <c r="C91" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D91" t="s">
         <v>55</v>
@@ -6733,7 +6733,7 @@
         <v>55</v>
       </c>
       <c r="C94" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D94" t="s">
         <v>55</v>
@@ -6851,7 +6851,7 @@
         <v>55</v>
       </c>
       <c r="C96" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D96" t="s">
         <v>55</v>
@@ -6910,7 +6910,7 @@
         <v>55</v>
       </c>
       <c r="C97" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D97" t="s">
         <v>55</v>
@@ -6969,7 +6969,7 @@
         <v>55</v>
       </c>
       <c r="C98" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D98" t="s">
         <v>55</v>
@@ -7087,7 +7087,7 @@
         <v>55</v>
       </c>
       <c r="C100" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D100" t="s">
         <v>55</v>
@@ -7264,7 +7264,7 @@
         <v>55</v>
       </c>
       <c r="C103" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D103" t="s">
         <v>55</v>
@@ -7294,7 +7294,7 @@
         <v>55</v>
       </c>
       <c r="M103" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N103" t="s">
         <v>55</v>
@@ -7438,7 +7438,7 @@
         <v>101</v>
       </c>
       <c r="B106" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C106" t="s">
         <v>55</v>
@@ -7733,7 +7733,7 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C111" t="s">
         <v>55</v>
@@ -7934,7 +7934,7 @@
         <v>55</v>
       </c>
       <c r="J114" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="K114" t="s">
         <v>55</v>
@@ -7993,7 +7993,7 @@
         <v>55</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K115" s="5" t="s">
         <v>55</v>
@@ -8011,16 +8011,16 @@
         <v>55</v>
       </c>
       <c r="P115" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="Q115" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R115" s="5" t="s">
         <v>12</v>
       </c>
       <c r="S115" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.35">
@@ -8052,7 +8052,7 @@
         <v>55</v>
       </c>
       <c r="J116" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K116" s="5" t="s">
         <v>55</v>
@@ -8070,16 +8070,16 @@
         <v>55</v>
       </c>
       <c r="P116" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="Q116" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R116" s="5" t="s">
         <v>12</v>
       </c>
       <c r="S116" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to match GUM build bot
</commit_message>
<xml_diff>
--- a/_build/utils/dm-dependencies/resources/non_dm_rules.xlsx
+++ b/_build/utils/dm-dependencies/resources/non_dm_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Corpora\GUM\GENTLE\repo\_build\utils\dm-dependencies\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA5E7FB-EAC6-473B-B4D4-80D6A72D127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0F80A4-2BB4-4A5E-8662-6895E22EF21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BF4EFA19-1866-4339-A4F4-33A768915554}"/>
+    <workbookView xWindow="6830" yWindow="340" windowWidth="18770" windowHeight="14520" xr2:uid="{BF4EFA19-1866-4339-A4F4-33A768915554}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1042,7 +1042,7 @@
     <t>$attrib_verb = (accept|acknowledge|add|admit|afraid|agree|announce|argue|ask|assert|assess|assume|assure|aware|believe|bet|call|care|certain|chant|check|claim|comment|complain|concern|conclude|confirm|convince|cry|decide|declare|determine|disappoint|discover|discuss|doubt|dream|emphasize|ensure|establish|estimate|exclaim|expect|explain|express|feel|figure|find|forget|gather|glad|guarantee|guess|happy|hear|hold|hope|hypothesize|imagine|implore|imply|indicate|inform|know|learn|lie|maintain|mean|mention|mindful|mutter|note|notice|observe|pant|perceive|point|posit|pray|predict|presume|promise|propose|proud|quote|quoth|re-iterate|read|realise|realize|reason|recall|recognize|recommend|reiterate|remember|remind|repeat|reply|report|resent|reveal|rule|say|scream|see|shout|show|shriek|shrug|sing|snap|start|state|stunned|suggest|summarize|suppose|sure|surprise|surprised|suspect|swear|tell|terrify|think|trust|tweet|understand|vlog|whisper|wish|witness|wonder|worry|write|be%like|go%say|keep%mind|bear%mind|make%sure)</t>
   </si>
   <si>
-    <t>(accurate|aggressive|amaze|amazing|attractive|awesome|awful|bad|beautiful|big|cathartic|cautionary|clean|clear|complicated|considerable|cool|correct|crazy|critical|cute|dark|decent|different|difficult|dreadful|easy|efficient|enough|essential|excellent|excited|exciting|false|fantastic|fine|frightful|froughtful|frustrate|fun|fundamental|funny|glad|goddamn|good|great|gross|happy|hard|heady|healthy|heartwarming|high|historic|honest|ideal|important|inaccurate|incorrect|insane|interesting|large|legendary|likely|long|low|lucky|magnificent|militant|natural|necessary|needy|nice|normal|okay|peaceful|perfect|pleasant|possible|practical|pretty|proud|rare|real|realistic|reliable|remarkable|right|sad|safe|same|scared|scary|scenic|significant|simple|small|smart|solid|sorry|special|strange|strong|stun|stunned|stupid|sure|surpries|surprising|sweet|tame|tired|toxic|trash|tremendous|true|unbelievable|unlikely|unnatural|unpalatable|unprecedented|useful|valuable|versatile|violent|warm|weird|wild|wild|wonderful|worth|wrong)</t>
+    <t>(accurate|aggressive|amaze|amazing|attractive|awesome|awful|bad|beautiful|big|cathartic|cautionary|clean|clear|commendable|complicated|considerable|cool|correct|crazy|critical|cute|dark|decent|different|difficult|dreadful|easy|efficient|enough|essential|excellent|excited|exciting|false|fantastic|fine|frightful|froughtful|frustrate|fun|fundamental|funny|glad|goddamn|good|great|gross|happy|hard|heady|healthy|heartwarming|high|historic|honest|ideal|important|inaccurate|incorrect|insane|interesting|large|legendary|likely|long|low|lucky|magnificent|militant|natural|necessary|needy|nice|normal|okay|peaceful|perfect|pleasant|possible|practical|pretty|proud|rare|real|realistic|reliable|remarkable|right|sad|safe|same|scared|scary|scenic|significant|simple|small|smart|solid|sorry|special|strange|strong|stun|stunned|stupid|sure|surpries|surprising|sweet|tame|tired|toxic|trash|tremendous|true|unbelievable|unlikely|unnatural|unpalatable|unprecedented|useful|valuable|versatile|violent|warm|weird|wild|wild|wonderful|worth|wrong)</t>
   </si>
 </sst>
 </file>

</xml_diff>